<commit_message>
Adding translations to dutch for the carrot fly
</commit_message>
<xml_diff>
--- a/i18n/excel_to_translation/uk.WarwickHRI.xlsx
+++ b/i18n/excel_to_translation/uk.WarwickHRI.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\development\ipm\ipm-decisions-meta-data\DSS-Metadata\i18n\excel_to_translation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{024933BB-90DC-48FE-B898-327FC1887A7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -13,12 +19,12 @@
     <sheet name="MELIAE_WarwickHRI" sheetId="4" r:id="rId4"/>
     <sheet name="PSILRO_WarwickHRI" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="377" uniqueCount="233">
   <si>
     <t>KEY</t>
   </si>
@@ -721,12 +727,33 @@
   <si>
     <t>Estimates the timing of Carrot Fly activity</t>
   </si>
+  <si>
+    <t>DE PLAAG: De wortelvlieg (Psila rosae/Chamaepsila rosae) overwintert in de grond als pop of als larve. Laat ontwikkelde insecten blijven als larven achter en voeden zich met wortels gedurende de winter. De insecten die overwinteren als larven vormen poppen in de lente. Uit beide soorten poppen komen vervolgens volwassen vliegen. De vrouwelijke vliegen leggen eitjes in de grond in de buurt van wortels en nadat ze zijn uitgekomen, voeden de larven zich met de wortels en graven er tunnels in, waardoor ze schade veroorzaken. Deze larven vormen poppen die leiden tot het uitkomen van een nieuwe generatie volwassenen. Afhankelijk van het lokale klimaat kan het aantal generaties van de wortelvlieg en de vluchten verschillen. Als het bijzonder warm weer is, kunnen de poppen van de wortelvlieg in rust gaan.DE BESLISSING: Het model voorspelt het ontluiken van de adulten en de ei-afleg doorheen het jaar. Dit maakt het voor de teler mogelijk om gericht te monitoren en risico verlagende acties te nemen om schade te beperkten. DE PARAMETERS: Het voorspellingsmodel voor wortelvlieg heeft de bodemtemperatuur op ongeveer 6 cm en luchttemperatuur op uurbasis nodig voor een goede voorspelling.REGIO: Dit model werd aangepast op basis van werk uitgevoerd in het VK. Klimaatdata is gevalideerd voor Vlaanderen.Selecteer ‘Parameters bewerken’ en selecteer de meest geschikte locatie voor jouw boerderij. De startdatum voor het model is 1 februari, omdat dit vaak de koudste periode van het jaar is.</t>
+  </si>
+  <si>
+    <t>Cumulatieve ontluiking generatie 1</t>
+  </si>
+  <si>
+    <t>Cumulatieve ontluiking generatie 2</t>
+  </si>
+  <si>
+    <t>Cumulatieve ontluiking generatie 3</t>
+  </si>
+  <si>
+    <t>Ei-leg generatie 1 (cumulatief)</t>
+  </si>
+  <si>
+    <t>Ei-leg generatie 2 (cumulatief)</t>
+  </si>
+  <si>
+    <t>Ei-leg generatie 3 (cumulatief)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -789,13 +816,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -833,7 +868,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -867,6 +902,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -901,9 +937,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1076,14 +1113,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1133,7 +1172,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -1189,14 +1228,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="95.734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="255.578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1246,7 +1291,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1254,7 +1299,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>19</v>
       </c>
@@ -1262,7 +1307,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>20</v>
       </c>
@@ -1270,7 +1315,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -1278,7 +1323,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -1286,7 +1331,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>23</v>
       </c>
@@ -1294,7 +1339,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>24</v>
       </c>
@@ -1302,7 +1347,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -1310,7 +1355,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -1318,7 +1363,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1326,7 +1371,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>28</v>
       </c>
@@ -1334,7 +1379,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>29</v>
       </c>
@@ -1342,7 +1387,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>30</v>
       </c>
@@ -1350,7 +1395,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -1358,7 +1403,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>32</v>
       </c>
@@ -1366,7 +1411,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>33</v>
       </c>
@@ -1374,7 +1419,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1382,7 +1427,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>35</v>
       </c>
@@ -1390,7 +1435,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>36</v>
       </c>
@@ -1398,7 +1443,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>37</v>
       </c>
@@ -1406,7 +1451,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>38</v>
       </c>
@@ -1414,7 +1459,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>39</v>
       </c>
@@ -1422,7 +1467,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>40</v>
       </c>
@@ -1430,7 +1475,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>41</v>
       </c>
@@ -1438,7 +1483,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>42</v>
       </c>
@@ -1446,7 +1491,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>43</v>
       </c>
@@ -1454,17 +1499,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>46</v>
       </c>
@@ -1472,7 +1517,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>47</v>
       </c>
@@ -1480,7 +1525,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>48</v>
       </c>
@@ -1488,7 +1533,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>49</v>
       </c>
@@ -1496,7 +1541,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>50</v>
       </c>
@@ -1504,7 +1549,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>51</v>
       </c>
@@ -1512,7 +1557,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>52</v>
       </c>
@@ -1520,7 +1565,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>53</v>
       </c>
@@ -1528,7 +1573,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>54</v>
       </c>
@@ -1542,14 +1587,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1599,7 +1644,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>81</v>
       </c>
@@ -1607,7 +1652,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>82</v>
       </c>
@@ -1615,7 +1660,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>83</v>
       </c>
@@ -1623,7 +1668,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>84</v>
       </c>
@@ -1631,7 +1676,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>85</v>
       </c>
@@ -1639,7 +1684,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>86</v>
       </c>
@@ -1647,7 +1692,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>87</v>
       </c>
@@ -1655,7 +1700,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>88</v>
       </c>
@@ -1663,7 +1708,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>89</v>
       </c>
@@ -1671,7 +1716,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>90</v>
       </c>
@@ -1679,7 +1724,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>91</v>
       </c>
@@ -1687,7 +1732,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>92</v>
       </c>
@@ -1695,7 +1740,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>93</v>
       </c>
@@ -1703,7 +1748,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>94</v>
       </c>
@@ -1711,7 +1756,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>95</v>
       </c>
@@ -1719,7 +1764,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>96</v>
       </c>
@@ -1727,7 +1772,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>97</v>
       </c>
@@ -1735,7 +1780,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>98</v>
       </c>
@@ -1743,7 +1788,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>99</v>
       </c>
@@ -1751,7 +1796,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>100</v>
       </c>
@@ -1759,7 +1804,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>101</v>
       </c>
@@ -1767,17 +1812,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>104</v>
       </c>
@@ -1785,7 +1830,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>105</v>
       </c>
@@ -1793,7 +1838,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>106</v>
       </c>
@@ -1801,7 +1846,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>107</v>
       </c>
@@ -1809,7 +1854,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>108</v>
       </c>
@@ -1817,7 +1862,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>109</v>
       </c>
@@ -1825,7 +1870,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>110</v>
       </c>
@@ -1833,7 +1878,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>111</v>
       </c>
@@ -1841,7 +1886,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>112</v>
       </c>
@@ -1855,14 +1900,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1912,7 +1957,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>128</v>
       </c>
@@ -1920,7 +1965,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>129</v>
       </c>
@@ -1928,7 +1973,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>130</v>
       </c>
@@ -1936,7 +1981,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>131</v>
       </c>
@@ -1944,7 +1989,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>132</v>
       </c>
@@ -1952,7 +1997,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>133</v>
       </c>
@@ -1960,7 +2005,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>134</v>
       </c>
@@ -1968,7 +2013,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>135</v>
       </c>
@@ -1976,7 +2021,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>136</v>
       </c>
@@ -1984,7 +2029,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>137</v>
       </c>
@@ -1992,7 +2037,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>138</v>
       </c>
@@ -2000,7 +2045,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>139</v>
       </c>
@@ -2008,7 +2053,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>140</v>
       </c>
@@ -2016,7 +2061,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>141</v>
       </c>
@@ -2024,7 +2069,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>142</v>
       </c>
@@ -2032,7 +2077,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>143</v>
       </c>
@@ -2040,7 +2085,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:2">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>144</v>
       </c>
@@ -2048,7 +2093,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="19" spans="1:2">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>145</v>
       </c>
@@ -2056,7 +2101,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>146</v>
       </c>
@@ -2064,7 +2109,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="21" spans="1:2">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>147</v>
       </c>
@@ -2072,7 +2117,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>148</v>
       </c>
@@ -2080,17 +2125,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>151</v>
       </c>
@@ -2098,7 +2143,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>152</v>
       </c>
@@ -2106,7 +2151,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>153</v>
       </c>
@@ -2114,7 +2159,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>154</v>
       </c>
@@ -2122,7 +2167,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>155</v>
       </c>
@@ -2130,7 +2175,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>156</v>
       </c>
@@ -2138,7 +2183,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>157</v>
       </c>
@@ -2146,7 +2191,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>158</v>
       </c>
@@ -2154,7 +2199,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>159</v>
       </c>
@@ -2168,14 +2213,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:P38"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2225,15 +2272,18 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>178</v>
       </c>
       <c r="B2" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="E2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>179</v>
       </c>
@@ -2241,7 +2291,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>180</v>
       </c>
@@ -2249,7 +2299,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>181</v>
       </c>
@@ -2257,7 +2307,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>182</v>
       </c>
@@ -2265,7 +2315,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="7" spans="1:16">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -2273,7 +2323,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -2281,7 +2331,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>185</v>
       </c>
@@ -2289,103 +2339,139 @@
         <v>218</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>186</v>
       </c>
       <c r="B10" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="E10" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>187</v>
       </c>
       <c r="B11" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="E11" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>188</v>
       </c>
       <c r="B12" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="E12" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>189</v>
       </c>
       <c r="B13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="E13" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>190</v>
       </c>
       <c r="B14" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="E14" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>191</v>
       </c>
       <c r="B15" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="E15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>192</v>
       </c>
       <c r="B16" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="E16" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>193</v>
       </c>
       <c r="B17" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="E17" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>194</v>
       </c>
       <c r="B18" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="E18" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>195</v>
       </c>
       <c r="B19" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="E19" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>196</v>
       </c>
       <c r="B20" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="E20" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>197</v>
       </c>
       <c r="B21" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="E21" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>198</v>
       </c>
@@ -2393,7 +2479,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>199</v>
       </c>
@@ -2401,7 +2487,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="24" spans="1:2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>200</v>
       </c>
@@ -2409,7 +2495,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="25" spans="1:2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>201</v>
       </c>
@@ -2417,7 +2503,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="26" spans="1:2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>202</v>
       </c>
@@ -2425,7 +2511,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="27" spans="1:2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>203</v>
       </c>
@@ -2433,17 +2519,17 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="29" spans="1:2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="30" spans="1:2">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>206</v>
       </c>
@@ -2451,7 +2537,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="31" spans="1:2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>207</v>
       </c>
@@ -2459,7 +2545,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="32" spans="1:2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>208</v>
       </c>
@@ -2467,7 +2553,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="33" spans="1:2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>209</v>
       </c>
@@ -2475,7 +2561,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="34" spans="1:2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>210</v>
       </c>
@@ -2483,7 +2569,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="35" spans="1:2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" t="s">
         <v>211</v>
       </c>
@@ -2491,7 +2577,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" t="s">
         <v>212</v>
       </c>
@@ -2499,7 +2585,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" t="s">
         <v>213</v>
       </c>
@@ -2507,7 +2593,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" t="s">
         <v>214</v>
       </c>

</xml_diff>